<commit_message>
A bit of BFO
</commit_message>
<xml_diff>
--- a/Submission/ArtifactsInProcess/ThreatRiskFoundationalTeminology.xlsx
+++ b/Submission/ArtifactsInProcess/ThreatRiskFoundationalTeminology.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="125">
   <si>
     <t>Anything</t>
   </si>
@@ -211,9 +211,6 @@
   </si>
   <si>
     <t>Has person and organization elements</t>
-  </si>
-  <si>
-    <t>UMLAction</t>
   </si>
   <si>
     <t>An Action is the fundamental unit of behavior specification in UML. An Action may take a set of inputs and produce a set of outputs, though either or both of these sets may be empty. Some Actions may modify the state of the system in which the Action executes.</t>
@@ -311,30 +308,15 @@
     <t>Object</t>
   </si>
   <si>
-    <t>Logic: Endurant</t>
-  </si>
-  <si>
-    <t>UML: ModelElement,  STIX-Python:object, DOLCE: Entity</t>
-  </si>
-  <si>
     <t>OWL:Thing, STIX:Entity, DOLCE: (not quality)</t>
   </si>
   <si>
     <t>SUMO: Temporal, DOLCE: Perdurant / Occurance</t>
   </si>
   <si>
-    <t>DOLCE: Non physical endurant?</t>
-  </si>
-  <si>
-    <t>UML: Event, DOCE: Event</t>
-  </si>
-  <si>
     <t>UML: State, OntoUML: Phase, DOLCE: State</t>
   </si>
   <si>
-    <t>DOLCE: Physical region</t>
-  </si>
-  <si>
     <t>Oasis xPRL:Party, DOLCE: Social Agent</t>
   </si>
   <si>
@@ -374,12 +356,6 @@
     <t>Relationship</t>
   </si>
   <si>
-    <t>A pattern, configuration or type of things that may exist (disjoint with template)</t>
-  </si>
-  <si>
-    <t>UML: Association end (partion match)</t>
-  </si>
-  <si>
     <t>UML:Namespace &amp; Type (Partial matchs)</t>
   </si>
   <si>
@@ -408,6 +384,36 @@
   </si>
   <si>
     <t>Process</t>
+  </si>
+  <si>
+    <t>UML: ModelElement,  STIX-Python:object, DOLCE: Entity, BFO:Entity</t>
+  </si>
+  <si>
+    <t>DOLCE: Non physical endurant?, BFO: Spatiotemporal Region</t>
+  </si>
+  <si>
+    <t>Logic: Endurant, BFO: Independent Continuant</t>
+  </si>
+  <si>
+    <t>BFO: Material Object</t>
+  </si>
+  <si>
+    <t>UML: Event, DOCE: Event, BFO: P{rocess Boundary</t>
+  </si>
+  <si>
+    <t>UMLAction, BFO: Process?</t>
+  </si>
+  <si>
+    <t>UML: Association end (partion match), BFO:Role</t>
+  </si>
+  <si>
+    <t>DOLCE: Physical region, BFO: Spatial Region</t>
+  </si>
+  <si>
+    <t>BFO: Subtype of Object</t>
+  </si>
+  <si>
+    <t>A pattern, configuration  of things that may exist (disjoint with actuality)</t>
   </si>
 </sst>
 </file>
@@ -551,6 +557,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1837465</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>18548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="29718000"/>
+          <a:ext cx="6885715" cy="4019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -843,9 +892,9 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <pane xSplit="1650" activePane="topRight"/>
+      <pane xSplit="1650" topLeftCell="B1" activePane="topRight"/>
       <selection activeCell="A22" sqref="A22:XFD22"/>
-      <selection pane="topRight" activeCell="K26" sqref="K26"/>
+      <selection pane="topRight" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,13 +921,13 @@
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="15"/>
       <c r="G1" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="15"/>
@@ -933,27 +982,27 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="M3" s="1" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="135" x14ac:dyDescent="0.25">
@@ -967,7 +1016,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="150" x14ac:dyDescent="0.25">
@@ -987,13 +1036,13 @@
         <v>54</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="75" x14ac:dyDescent="0.25">
@@ -1010,10 +1059,10 @@
         <v>1</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="105" x14ac:dyDescent="0.25">
@@ -1039,7 +1088,7 @@
         <v>49</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="210" x14ac:dyDescent="0.25">
@@ -1062,7 +1111,7 @@
         <v>40</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>36</v>
@@ -1091,15 +1140,15 @@
         <v>41</v>
       </c>
       <c r="M10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -1108,10 +1157,10 @@
         <v>24</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -1125,10 +1174,10 @@
         <v>1</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="90" x14ac:dyDescent="0.25">
@@ -1157,7 +1206,7 @@
         <v>38</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>64</v>
@@ -1165,7 +1214,7 @@
     </row>
     <row r="14" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>46</v>
@@ -1191,7 +1240,7 @@
         <v>8</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>6</v>
@@ -1217,7 +1266,7 @@
         <v>9</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>44</v>
@@ -1248,7 +1297,10 @@
         <v>6</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="60" x14ac:dyDescent="0.25">
@@ -1256,7 +1308,7 @@
         <v>42</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>21</v>
@@ -1277,15 +1329,15 @@
         <v>43</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>20</v>
@@ -1300,21 +1352,24 @@
         <v>59</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="210" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C21" t="s">
         <v>39</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>48</v>
@@ -1323,7 +1378,7 @@
         <v>50</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="60" x14ac:dyDescent="0.25">
@@ -1334,7 +1389,7 @@
         <v>61</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>3</v>
@@ -1343,13 +1398,13 @@
         <v>61</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>61</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>61</v>
@@ -1360,33 +1415,33 @@
     </row>
     <row r="23" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>1</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="75" x14ac:dyDescent="0.25">
@@ -1397,30 +1452,30 @@
         <v>11</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>119</v>
+        <v>96</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>2</v>
@@ -1428,13 +1483,13 @@
     </row>
     <row r="27" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C27" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>2</v>
@@ -1442,27 +1497,28 @@
     </row>
     <row r="28" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>118</v>
+      <c r="G28" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>